<commit_message>
Fixed small issue with submit windows not closing
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/ZABARS.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/ZABARS.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,32 @@
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>r1ange white angel hair 6/16-oz $  16.02 1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1 01ANGE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>r1ling white linguini 6/16-oz $  16.02 2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2 01LING</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>